<commit_message>
add Suppl. files 3 & 4
</commit_message>
<xml_diff>
--- a/suppl_files/supplementary_file2.xlsx
+++ b/suppl_files/supplementary_file2.xlsx
@@ -34,12 +34,12 @@
     <t xml:space="preserve">exo-turquoise</t>
   </si>
   <si>
+    <t xml:space="preserve">TAGLN2</t>
+  </si>
+  <si>
     <t xml:space="preserve">BEX3</t>
   </si>
   <si>
-    <t xml:space="preserve">TAGLN2</t>
-  </si>
-  <si>
     <t xml:space="preserve">GFI1B</t>
   </si>
   <si>
@@ -49,136 +49,136 @@
     <t xml:space="preserve">CMIP</t>
   </si>
   <si>
+    <t xml:space="preserve">TLK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIMS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIF4G3</t>
+  </si>
+  <si>
     <t xml:space="preserve">PHKB</t>
   </si>
   <si>
-    <t xml:space="preserve">EIF4G3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIMS1</t>
-  </si>
-  <si>
     <t xml:space="preserve">MTURN</t>
   </si>
   <si>
+    <t xml:space="preserve">GRAP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAXDC2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITGB1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YWHAZ</t>
+  </si>
+  <si>
     <t xml:space="preserve">HOOK3</t>
   </si>
   <si>
-    <t xml:space="preserve">FAXDC2</t>
+    <t xml:space="preserve">STON2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUSD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESAM</t>
   </si>
   <si>
     <t xml:space="preserve">MAP3K5</t>
   </si>
   <si>
-    <t xml:space="preserve">YWHAZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ITGB1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRAP2</t>
+    <t xml:space="preserve">CD226</t>
   </si>
   <si>
     <t xml:space="preserve">NAP1L1</t>
   </si>
   <si>
-    <t xml:space="preserve">SUSD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STON2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESAM</t>
+    <t xml:space="preserve">ASAH1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTPN12</t>
   </si>
   <si>
     <t xml:space="preserve">ITFG1</t>
   </si>
   <si>
-    <t xml:space="preserve">PTPN12</t>
+    <t xml:space="preserve">MOB1B</t>
   </si>
   <si>
     <t xml:space="preserve">MPP1</t>
   </si>
   <si>
-    <t xml:space="preserve">ASAH1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOB1B</t>
+    <t xml:space="preserve">SKAP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCGF5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2AC6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITM2B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACRBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANO6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFSD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LRBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIF2AK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNAP23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEPROT</t>
   </si>
   <si>
     <t xml:space="preserve">ETFA</t>
   </si>
   <si>
-    <t xml:space="preserve">CD226</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKAP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EIF2AK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2AC6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNAP23</t>
-  </si>
-  <si>
     <t xml:space="preserve">NLK</t>
   </si>
   <si>
-    <t xml:space="preserve">ITM2B</t>
+    <t xml:space="preserve">SMIM3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KCTD20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPRE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAM1</t>
   </si>
   <si>
     <t xml:space="preserve">PAIP2</t>
   </si>
   <si>
-    <t xml:space="preserve">ACRBP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NBAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MFSD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPTN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCGF5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KMT2C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEPROT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KCTD20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LRBA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGS10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANO6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAPRE2</t>
+    <t xml:space="preserve">KIF2A</t>
   </si>
   <si>
     <t xml:space="preserve">DCAF12</t>
@@ -193,159 +193,159 @@
     <t xml:space="preserve">MXI1</t>
   </si>
   <si>
+    <t xml:space="preserve">FAM210B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TENT5C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOXO3</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALAS2</t>
   </si>
   <si>
-    <t xml:space="preserve">FAM210B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOXO3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TENT5C</t>
+    <t xml:space="preserve">GYPC</t>
   </si>
   <si>
     <t xml:space="preserve">BAG1</t>
   </si>
   <si>
-    <t xml:space="preserve">GYPC</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPIA</t>
   </si>
   <si>
     <t xml:space="preserve">SLC4A1</t>
   </si>
   <si>
+    <t xml:space="preserve">SLC25A39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MKRN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HBA2</t>
+  </si>
+  <si>
     <t xml:space="preserve">MICAL2</t>
   </si>
   <si>
-    <t xml:space="preserve">SLC25A39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MKRN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HBA2</t>
-  </si>
-  <si>
     <t xml:space="preserve">MARCHF8</t>
   </si>
   <si>
+    <t xml:space="preserve">HBA1</t>
+  </si>
+  <si>
     <t xml:space="preserve">TMOD1</t>
   </si>
   <si>
-    <t xml:space="preserve">HBA1</t>
-  </si>
-  <si>
     <t xml:space="preserve">RANBP10</t>
   </si>
   <si>
+    <t xml:space="preserve">MARK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSMF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHOSPHO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLC14A1</t>
+  </si>
+  <si>
     <t xml:space="preserve">TFDP1</t>
   </si>
   <si>
-    <t xml:space="preserve">SLC14A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PSMF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHOSPHO1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARK3</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASCC2</t>
   </si>
   <si>
+    <t xml:space="preserve">NFIX</t>
+  </si>
+  <si>
     <t xml:space="preserve">GLRX5</t>
   </si>
   <si>
-    <t xml:space="preserve">NFIX</t>
+    <t xml:space="preserve">TSPAN5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRADB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELENBP1</t>
   </si>
   <si>
     <t xml:space="preserve">YBX3</t>
   </si>
   <si>
-    <t xml:space="preserve">TSPAN5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELENBP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRADB</t>
+    <t xml:space="preserve">RNF123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNF10</t>
   </si>
   <si>
     <t xml:space="preserve">JAZF1</t>
   </si>
   <si>
+    <t xml:space="preserve">CISD2</t>
+  </si>
+  <si>
     <t xml:space="preserve">GCLC</t>
   </si>
   <si>
-    <t xml:space="preserve">RNF123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CISD2</t>
+    <t xml:space="preserve">PLCL2</t>
   </si>
   <si>
     <t xml:space="preserve">GSPT1</t>
   </si>
   <si>
+    <t xml:space="preserve">BCL2L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPR146</t>
+  </si>
+  <si>
     <t xml:space="preserve">RBM38</t>
   </si>
   <si>
-    <t xml:space="preserve">GPR146</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLCL2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNF10</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHPT1</t>
   </si>
   <si>
     <t xml:space="preserve">HAGH</t>
   </si>
   <si>
-    <t xml:space="preserve">BCL2L1</t>
+    <t xml:space="preserve">ABALON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IFIT1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAM104A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP2K3</t>
   </si>
   <si>
     <t xml:space="preserve">C9orf40</t>
   </si>
   <si>
-    <t xml:space="preserve">ABALON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFIT1B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C9orf78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WNK1</t>
-  </si>
-  <si>
     <t xml:space="preserve">DNAH14</t>
   </si>
   <si>
     <t xml:space="preserve">exo-blue</t>
   </si>
   <si>
+    <t xml:space="preserve">FMNL1</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEPTIN9</t>
   </si>
   <si>
-    <t xml:space="preserve">FMNL1</t>
-  </si>
-  <si>
     <t xml:space="preserve">ARHGDIA</t>
   </si>
   <si>
@@ -358,133 +358,133 @@
     <t xml:space="preserve">AKNA</t>
   </si>
   <si>
+    <t xml:space="preserve">CYFIP2</t>
+  </si>
+  <si>
     <t xml:space="preserve">INPP5D</t>
   </si>
   <si>
-    <t xml:space="preserve">CYFIP2</t>
+    <t xml:space="preserve">ARHGAP9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CORO1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRK2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELF4</t>
   </si>
   <si>
     <t xml:space="preserve">ADAP1</t>
   </si>
   <si>
-    <t xml:space="preserve">ARHGAP9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CORO1A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRK2</t>
+    <t xml:space="preserve">KIF21B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREX1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEF6</t>
   </si>
   <si>
     <t xml:space="preserve">NUMA1</t>
   </si>
   <si>
+    <t xml:space="preserve">STK10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PKN1</t>
+  </si>
+  <si>
     <t xml:space="preserve">CCAR2</t>
   </si>
   <si>
-    <t xml:space="preserve">PKN1</t>
+    <t xml:space="preserve">ARHGEF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOB3A</t>
   </si>
   <si>
     <t xml:space="preserve">CSK</t>
   </si>
   <si>
-    <t xml:space="preserve">ELF4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIF21B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEF6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PREX1</t>
+    <t xml:space="preserve">MYO1G</t>
   </si>
   <si>
     <t xml:space="preserve">CERK</t>
   </si>
   <si>
-    <t xml:space="preserve">STK10</t>
-  </si>
-  <si>
     <t xml:space="preserve">KIAA0930</t>
   </si>
   <si>
-    <t xml:space="preserve">MYO1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOB3A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARHGEF1</t>
-  </si>
-  <si>
     <t xml:space="preserve">BRD1</t>
   </si>
   <si>
+    <t xml:space="preserve">SASH3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCDC69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KLF13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EHMT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARD11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYTH1</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIPA1</t>
   </si>
   <si>
-    <t xml:space="preserve">EHMT2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SASH3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYTH1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KLF13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCDC69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CARD11</t>
+    <t xml:space="preserve">ATXN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCL9L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLLT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUNX3</t>
   </si>
   <si>
     <t xml:space="preserve">RABL6</t>
   </si>
   <si>
+    <t xml:space="preserve">EFHD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRD2</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSNK1G2</t>
   </si>
   <si>
-    <t xml:space="preserve">ATXN1</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRKCSH</t>
   </si>
   <si>
-    <t xml:space="preserve">BRD2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCL9L</t>
-  </si>
-  <si>
     <t xml:space="preserve">ANKFY1</t>
   </si>
   <si>
-    <t xml:space="preserve">MLLT6</t>
+    <t xml:space="preserve">VPS16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLE5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INTS1</t>
   </si>
   <si>
     <t xml:space="preserve">OGDH</t>
   </si>
   <si>
-    <t xml:space="preserve">INTS1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EFHD2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VPS16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RUNX3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUBP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLE5</t>
+    <t xml:space="preserve">JADE2</t>
   </si>
   <si>
     <t xml:space="preserve">AKAP7</t>
@@ -493,21 +493,21 @@
     <t xml:space="preserve">exo-yellow</t>
   </si>
   <si>
+    <t xml:space="preserve">SWT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DCUN1D1</t>
+  </si>
+  <si>
     <t xml:space="preserve">PICALM</t>
   </si>
   <si>
-    <t xml:space="preserve">SWT1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCUN1D1</t>
+    <t xml:space="preserve">USP12</t>
   </si>
   <si>
     <t xml:space="preserve">KIAA1586</t>
   </si>
   <si>
-    <t xml:space="preserve">USP12</t>
-  </si>
-  <si>
     <t xml:space="preserve">SUCO</t>
   </si>
   <si>
@@ -520,55 +520,64 @@
     <t xml:space="preserve">MBNL3</t>
   </si>
   <si>
+    <t xml:space="preserve">EPB41</t>
+  </si>
+  <si>
     <t xml:space="preserve">NPAT</t>
   </si>
   <si>
-    <t xml:space="preserve">EPB41</t>
+    <t xml:space="preserve">ISCA1</t>
   </si>
   <si>
     <t xml:space="preserve">CDC27</t>
   </si>
   <si>
+    <t xml:space="preserve">USP15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIF1B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCMTD1</t>
+  </si>
+  <si>
     <t xml:space="preserve">SLF1</t>
   </si>
   <si>
-    <t xml:space="preserve">ISCA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USP15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCMTD1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EIF1B</t>
-  </si>
-  <si>
     <t xml:space="preserve">TUBGCP2</t>
   </si>
   <si>
     <t xml:space="preserve">HAUS6</t>
   </si>
   <si>
+    <t xml:space="preserve">YIPF6</t>
+  </si>
+  <si>
     <t xml:space="preserve">FUS</t>
   </si>
   <si>
+    <t xml:space="preserve">BIRC2</t>
+  </si>
+  <si>
     <t xml:space="preserve">NADSYN1</t>
   </si>
   <si>
+    <t xml:space="preserve">AP3D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APEH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARL6IP1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ATXN2L</t>
   </si>
   <si>
-    <t xml:space="preserve">YIPF6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP3D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APEH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARL6IP1</t>
+    <t xml:space="preserve">PDXK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KNL1</t>
   </si>
   <si>
     <t xml:space="preserve">UBR2</t>
@@ -577,67 +586,58 @@
     <t xml:space="preserve">GTF2B</t>
   </si>
   <si>
-    <t xml:space="preserve">BIRC2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDXK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KNL1</t>
+    <t xml:space="preserve">SNCA</t>
   </si>
   <si>
     <t xml:space="preserve">PKN2</t>
   </si>
   <si>
+    <t xml:space="preserve">SCAF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARD10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KHSRP</t>
+  </si>
+  <si>
     <t xml:space="preserve">COPS2</t>
   </si>
   <si>
+    <t xml:space="preserve">SEC62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTN4</t>
+  </si>
+  <si>
     <t xml:space="preserve">DYNC1LI1</t>
   </si>
   <si>
-    <t xml:space="preserve">CARD10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCAF1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KHSRP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNCA</t>
-  </si>
-  <si>
     <t xml:space="preserve">YIF1A</t>
   </si>
   <si>
-    <t xml:space="preserve">ACTN4</t>
-  </si>
-  <si>
     <t xml:space="preserve">EIF3B</t>
   </si>
   <si>
+    <t xml:space="preserve">PPM1G</t>
+  </si>
+  <si>
     <t xml:space="preserve">SLC35A4</t>
   </si>
   <si>
+    <t xml:space="preserve">CEP135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEX10</t>
+  </si>
+  <si>
     <t xml:space="preserve">FDPS</t>
   </si>
   <si>
     <t xml:space="preserve">KNOP1</t>
   </si>
   <si>
-    <t xml:space="preserve">SEC62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CEP135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPM1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEX10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DPP9</t>
+    <t xml:space="preserve">NACC1</t>
   </si>
   <si>
     <t xml:space="preserve">RPL34</t>
@@ -655,12 +655,12 @@
     <t xml:space="preserve">RPL11</t>
   </si>
   <si>
+    <t xml:space="preserve">RPS11</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPS21</t>
   </si>
   <si>
-    <t xml:space="preserve">RPS11</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPL27A</t>
   </si>
   <si>
@@ -670,129 +670,129 @@
     <t xml:space="preserve">RPS6</t>
   </si>
   <si>
+    <t xml:space="preserve">RPS7</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPS27</t>
   </si>
   <si>
     <t xml:space="preserve">RPL24</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL27</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPL29</t>
   </si>
   <si>
-    <t xml:space="preserve">RPS7</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPL32</t>
   </si>
   <si>
-    <t xml:space="preserve">RPL27</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPLP1</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPL13A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPL37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS8</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPL38</t>
   </si>
   <si>
-    <t xml:space="preserve">RPL19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPL37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPL13A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS23</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPL23A</t>
   </si>
   <si>
     <t xml:space="preserve">RPL39</t>
   </si>
   <si>
+    <t xml:space="preserve">RPS16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPL23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEF1B2</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPS12</t>
   </si>
   <si>
-    <t xml:space="preserve">RPL23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEF1B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS13</t>
+    <t xml:space="preserve">RACK1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPSA</t>
   </si>
   <si>
     <t xml:space="preserve">RPS14</t>
   </si>
   <si>
+    <t xml:space="preserve">RPS28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPL7A</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPS25</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL30</t>
+  </si>
+  <si>
     <t xml:space="preserve">FAU</t>
   </si>
   <si>
-    <t xml:space="preserve">RPSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RACK1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPL30</t>
+    <t xml:space="preserve">RPS19</t>
   </si>
   <si>
     <t xml:space="preserve">RPS27A</t>
   </si>
   <si>
-    <t xml:space="preserve">RPS15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPS19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPL7A</t>
+    <t xml:space="preserve">RPL18</t>
   </si>
   <si>
     <t xml:space="preserve">RPS20</t>
   </si>
   <si>
-    <t xml:space="preserve">RPL18</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPL12</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL28</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPS15A</t>
   </si>
   <si>
-    <t xml:space="preserve">RPL28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPL37A</t>
-  </si>
-  <si>
     <t xml:space="preserve">RPL3</t>
   </si>
   <si>
+    <t xml:space="preserve">RPL14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPS5</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPL13</t>
   </si>
   <si>
-    <t xml:space="preserve">RPL14</t>
-  </si>
-  <si>
     <t xml:space="preserve">BNIP3L</t>
   </si>
   <si>
@@ -805,12 +805,12 @@
     <t xml:space="preserve">FBXO7</t>
   </si>
   <si>
+    <t xml:space="preserve">HEMGN</t>
+  </si>
+  <si>
     <t xml:space="preserve">NSUN3</t>
   </si>
   <si>
-    <t xml:space="preserve">HEMGN</t>
-  </si>
-  <si>
     <t xml:space="preserve">UBE2D3</t>
   </si>
   <si>
@@ -823,24 +823,24 @@
     <t xml:space="preserve">BPGM</t>
   </si>
   <si>
+    <t xml:space="preserve">TRIM23</t>
+  </si>
+  <si>
     <t xml:space="preserve">YOD1</t>
   </si>
   <si>
-    <t xml:space="preserve">TRIM23</t>
-  </si>
-  <si>
     <t xml:space="preserve">GYPB</t>
   </si>
   <si>
     <t xml:space="preserve">PCMTD2</t>
   </si>
   <si>
+    <t xml:space="preserve">RNF14</t>
+  </si>
+  <si>
     <t xml:space="preserve">TCP11L2</t>
   </si>
   <si>
-    <t xml:space="preserve">RNF14</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHD3</t>
   </si>
   <si>
@@ -862,52 +862,52 @@
     <t xml:space="preserve">TBCEL</t>
   </si>
   <si>
+    <t xml:space="preserve">ABCC13</t>
+  </si>
+  <si>
     <t xml:space="preserve">DNAJB4</t>
   </si>
   <si>
-    <t xml:space="preserve">ABCC13</t>
-  </si>
-  <si>
     <t xml:space="preserve">RBM12</t>
   </si>
   <si>
+    <t xml:space="preserve">POLR1D</t>
+  </si>
+  <si>
     <t xml:space="preserve">SAMD9</t>
   </si>
   <si>
-    <t xml:space="preserve">POLR1D</t>
+    <t xml:space="preserve">PTGES3</t>
   </si>
   <si>
     <t xml:space="preserve">NCOR2</t>
   </si>
   <si>
-    <t xml:space="preserve">PTGES3</t>
+    <t xml:space="preserve">WDR48</t>
   </si>
   <si>
     <t xml:space="preserve">ENSG00000234961</t>
   </si>
   <si>
-    <t xml:space="preserve">WDR48</t>
-  </si>
-  <si>
     <t xml:space="preserve">TMEM184B</t>
   </si>
   <si>
+    <t xml:space="preserve">SLC25A46</t>
+  </si>
+  <si>
     <t xml:space="preserve">PGPEP1</t>
   </si>
   <si>
-    <t xml:space="preserve">SLC25A46</t>
-  </si>
-  <si>
     <t xml:space="preserve">ERI1</t>
   </si>
   <si>
     <t xml:space="preserve">RGCC</t>
   </si>
   <si>
+    <t xml:space="preserve">GAPT</t>
+  </si>
+  <si>
     <t xml:space="preserve">TFDP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAPT</t>
   </si>
   <si>
     <t xml:space="preserve">PGAP6</t>
@@ -1276,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>749.710870617121</v>
+        <v>556.197718710502</v>
       </c>
     </row>
     <row r="3">
@@ -1287,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>740.58649022818</v>
+        <v>548.168008760217</v>
       </c>
     </row>
     <row r="4">
@@ -1298,7 +1298,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="n">
-        <v>739.901520667728</v>
+        <v>544.632366176061</v>
       </c>
     </row>
     <row r="5">
@@ -1309,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>729.11751971121</v>
+        <v>539.18018284233</v>
       </c>
     </row>
     <row r="6">
@@ -1320,7 +1320,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>727.587234893064</v>
+        <v>538.391981769415</v>
       </c>
     </row>
     <row r="7">
@@ -1331,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>726.064064841462</v>
+        <v>533.254459066852</v>
       </c>
     </row>
     <row r="8">
@@ -1342,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>724.07058836869</v>
+        <v>530.507108257452</v>
       </c>
     </row>
     <row r="9">
@@ -1353,7 +1353,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>721.248279158522</v>
+        <v>530.225297072104</v>
       </c>
     </row>
     <row r="10">
@@ -1364,7 +1364,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>720.398762375669</v>
+        <v>528.2152526879</v>
       </c>
     </row>
     <row r="11">
@@ -1375,7 +1375,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>717.223612502375</v>
+        <v>526.364715698304</v>
       </c>
     </row>
     <row r="12">
@@ -1386,7 +1386,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>715.812883269323</v>
+        <v>526.159769508328</v>
       </c>
     </row>
     <row r="13">
@@ -1397,7 +1397,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="n">
-        <v>713.890851571027</v>
+        <v>524.765240159902</v>
       </c>
     </row>
     <row r="14">
@@ -1408,7 +1408,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>713.256467529578</v>
+        <v>522.035792894117</v>
       </c>
     </row>
     <row r="15">
@@ -1419,7 +1419,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>712.072079678381</v>
+        <v>519.424550152628</v>
       </c>
     </row>
     <row r="16">
@@ -1430,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>709.049357529686</v>
+        <v>516.989616490855</v>
       </c>
     </row>
     <row r="17">
@@ -1441,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>708.362280483219</v>
+        <v>515.506255468624</v>
       </c>
     </row>
     <row r="18">
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>708.188855617937</v>
+        <v>514.628313532951</v>
       </c>
     </row>
     <row r="19">
@@ -1463,7 +1463,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>706.129771072411</v>
+        <v>514.604084183305</v>
       </c>
     </row>
     <row r="20">
@@ -1474,7 +1474,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>705.152463737363</v>
+        <v>514.274706157179</v>
       </c>
     </row>
     <row r="21">
@@ -1485,7 +1485,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="n">
-        <v>703.323641894723</v>
+        <v>507.931842573554</v>
       </c>
     </row>
     <row r="22">
@@ -1496,7 +1496,7 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
-        <v>701.98128967495</v>
+        <v>507.923733069181</v>
       </c>
     </row>
     <row r="23">
@@ -1507,7 +1507,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="n">
-        <v>698.873808090088</v>
+        <v>504.149997229695</v>
       </c>
     </row>
     <row r="24">
@@ -1518,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="n">
-        <v>694.822457114063</v>
+        <v>503.706390747907</v>
       </c>
     </row>
     <row r="25">
@@ -1529,7 +1529,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>694.809435551505</v>
+        <v>503.68109366964</v>
       </c>
     </row>
     <row r="26">
@@ -1540,7 +1540,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>694.429000241435</v>
+        <v>501.609650562961</v>
       </c>
     </row>
     <row r="27">
@@ -1551,7 +1551,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>692.625021592578</v>
+        <v>500.930050535055</v>
       </c>
     </row>
     <row r="28">
@@ -1562,7 +1562,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>689.695859873229</v>
+        <v>499.499271565557</v>
       </c>
     </row>
     <row r="29">
@@ -1573,7 +1573,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>689.308560313438</v>
+        <v>499.434616279847</v>
       </c>
     </row>
     <row r="30">
@@ -1584,7 +1584,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>688.941695186948</v>
+        <v>498.508302181787</v>
       </c>
     </row>
     <row r="31">
@@ -1595,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>688.363165072293</v>
+        <v>498.256698741006</v>
       </c>
     </row>
     <row r="32">
@@ -1606,7 +1606,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>686.120507314173</v>
+        <v>496.735243385615</v>
       </c>
     </row>
     <row r="33">
@@ -1617,7 +1617,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>684.67003326794</v>
+        <v>494.590272845758</v>
       </c>
     </row>
     <row r="34">
@@ -1628,7 +1628,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>683.789335064032</v>
+        <v>494.34160730653</v>
       </c>
     </row>
     <row r="35">
@@ -1639,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>682.842516675258</v>
+        <v>493.941181664089</v>
       </c>
     </row>
     <row r="36">
@@ -1650,7 +1650,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>682.023346938447</v>
+        <v>492.923521317764</v>
       </c>
     </row>
     <row r="37">
@@ -1661,7 +1661,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>681.726064532182</v>
+        <v>492.204053293729</v>
       </c>
     </row>
     <row r="38">
@@ -1672,7 +1672,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>681.582797395249</v>
+        <v>491.605112523113</v>
       </c>
     </row>
     <row r="39">
@@ -1683,7 +1683,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>681.408683573436</v>
+        <v>491.063128978742</v>
       </c>
     </row>
     <row r="40">
@@ -1694,7 +1694,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>681.221567309555</v>
+        <v>489.982118982202</v>
       </c>
     </row>
     <row r="41">
@@ -1705,7 +1705,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>681.132287343685</v>
+        <v>489.975218280218</v>
       </c>
     </row>
     <row r="42">
@@ -1716,7 +1716,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="n">
-        <v>680.816632743873</v>
+        <v>489.845095067237</v>
       </c>
     </row>
     <row r="43">
@@ -1727,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>679.748819730978</v>
+        <v>489.834724490322</v>
       </c>
     </row>
     <row r="44">
@@ -1738,7 +1738,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="n">
-        <v>679.374590434395</v>
+        <v>488.626133144278</v>
       </c>
     </row>
     <row r="45">
@@ -1749,7 +1749,7 @@
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>678.538573951259</v>
+        <v>487.875129459785</v>
       </c>
     </row>
     <row r="46">
@@ -1760,7 +1760,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>678.529186740353</v>
+        <v>486.622097252431</v>
       </c>
     </row>
     <row r="47">
@@ -1771,7 +1771,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>677.916868710225</v>
+        <v>485.819308223747</v>
       </c>
     </row>
     <row r="48">
@@ -1782,7 +1782,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>677.801990056804</v>
+        <v>484.778117348272</v>
       </c>
     </row>
     <row r="49">
@@ -1793,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>677.336953326536</v>
+        <v>484.05163276501</v>
       </c>
     </row>
     <row r="50">
@@ -1804,7 +1804,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>675.470509141874</v>
+        <v>483.905043429977</v>
       </c>
     </row>
     <row r="51">
@@ -1815,7 +1815,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>674.693137210115</v>
+        <v>482.806464708016</v>
       </c>
     </row>
   </sheetData>
@@ -1851,7 +1851,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="n">
-        <v>15.5331433655955</v>
+        <v>9.7247016627802</v>
       </c>
     </row>
     <row r="3">
@@ -1862,7 +1862,7 @@
         <v>55</v>
       </c>
       <c r="C3" t="n">
-        <v>15.1646981438017</v>
+        <v>9.4244630644741</v>
       </c>
     </row>
     <row r="4">
@@ -1873,7 +1873,7 @@
         <v>55</v>
       </c>
       <c r="C4" t="n">
-        <v>14.1100416008242</v>
+        <v>8.85214116929591</v>
       </c>
     </row>
     <row r="5">
@@ -1884,7 +1884,7 @@
         <v>55</v>
       </c>
       <c r="C5" t="n">
-        <v>13.0168671017252</v>
+        <v>8.02029447162387</v>
       </c>
     </row>
     <row r="6">
@@ -1895,7 +1895,7 @@
         <v>55</v>
       </c>
       <c r="C6" t="n">
-        <v>12.9821213925843</v>
+        <v>7.82080829250583</v>
       </c>
     </row>
     <row r="7">
@@ -1906,7 +1906,7 @@
         <v>55</v>
       </c>
       <c r="C7" t="n">
-        <v>12.9813653802786</v>
+        <v>7.81357971837627</v>
       </c>
     </row>
     <row r="8">
@@ -1917,7 +1917,7 @@
         <v>55</v>
       </c>
       <c r="C8" t="n">
-        <v>12.810249091262</v>
+        <v>7.73439498491641</v>
       </c>
     </row>
     <row r="9">
@@ -1928,7 +1928,7 @@
         <v>55</v>
       </c>
       <c r="C9" t="n">
-        <v>12.744182875507</v>
+        <v>7.56532255096082</v>
       </c>
     </row>
     <row r="10">
@@ -1939,7 +1939,7 @@
         <v>55</v>
       </c>
       <c r="C10" t="n">
-        <v>12.445001844346</v>
+        <v>7.4165666522855</v>
       </c>
     </row>
     <row r="11">
@@ -1950,7 +1950,7 @@
         <v>55</v>
       </c>
       <c r="C11" t="n">
-        <v>12.371372531364</v>
+        <v>7.31206827524504</v>
       </c>
     </row>
     <row r="12">
@@ -1961,7 +1961,7 @@
         <v>55</v>
       </c>
       <c r="C12" t="n">
-        <v>12.2794976887927</v>
+        <v>7.14430116677103</v>
       </c>
     </row>
     <row r="13">
@@ -1972,7 +1972,7 @@
         <v>55</v>
       </c>
       <c r="C13" t="n">
-        <v>11.9521495870418</v>
+        <v>7.03142549687411</v>
       </c>
     </row>
     <row r="14">
@@ -1983,7 +1983,7 @@
         <v>55</v>
       </c>
       <c r="C14" t="n">
-        <v>11.5653291730991</v>
+        <v>6.92368757827962</v>
       </c>
     </row>
     <row r="15">
@@ -1994,7 +1994,7 @@
         <v>55</v>
       </c>
       <c r="C15" t="n">
-        <v>11.5154517715594</v>
+        <v>6.77810033492838</v>
       </c>
     </row>
     <row r="16">
@@ -2005,7 +2005,7 @@
         <v>55</v>
       </c>
       <c r="C16" t="n">
-        <v>11.3206633129205</v>
+        <v>6.60728333400852</v>
       </c>
     </row>
     <row r="17">
@@ -2016,7 +2016,7 @@
         <v>55</v>
       </c>
       <c r="C17" t="n">
-        <v>11.164852524589</v>
+        <v>6.52777252450919</v>
       </c>
     </row>
     <row r="18">
@@ -2027,7 +2027,7 @@
         <v>55</v>
       </c>
       <c r="C18" t="n">
-        <v>10.9652488375116</v>
+        <v>6.14313318985327</v>
       </c>
     </row>
     <row r="19">
@@ -2038,7 +2038,7 @@
         <v>55</v>
       </c>
       <c r="C19" t="n">
-        <v>10.005404400115</v>
+        <v>5.65371989333633</v>
       </c>
     </row>
     <row r="20">
@@ -2049,7 +2049,7 @@
         <v>55</v>
       </c>
       <c r="C20" t="n">
-        <v>9.90384391681757</v>
+        <v>5.27064050075327</v>
       </c>
     </row>
     <row r="21">
@@ -2060,7 +2060,7 @@
         <v>55</v>
       </c>
       <c r="C21" t="n">
-        <v>9.53998424510623</v>
+        <v>5.16853548920184</v>
       </c>
     </row>
     <row r="22">
@@ -2071,7 +2071,7 @@
         <v>55</v>
       </c>
       <c r="C22" t="n">
-        <v>9.2691355250459</v>
+        <v>4.8935332775661</v>
       </c>
     </row>
     <row r="23">
@@ -2082,7 +2082,7 @@
         <v>55</v>
       </c>
       <c r="C23" t="n">
-        <v>9.00490370311707</v>
+        <v>4.87567333648197</v>
       </c>
     </row>
     <row r="24">
@@ -2093,7 +2093,7 @@
         <v>55</v>
       </c>
       <c r="C24" t="n">
-        <v>8.91040512196821</v>
+        <v>4.81772137569233</v>
       </c>
     </row>
     <row r="25">
@@ -2104,7 +2104,7 @@
         <v>55</v>
       </c>
       <c r="C25" t="n">
-        <v>8.90032108058979</v>
+        <v>4.81632799137259</v>
       </c>
     </row>
     <row r="26">
@@ -2115,7 +2115,7 @@
         <v>55</v>
       </c>
       <c r="C26" t="n">
-        <v>8.84378046396177</v>
+        <v>4.70822864014993</v>
       </c>
     </row>
     <row r="27">
@@ -2126,7 +2126,7 @@
         <v>55</v>
       </c>
       <c r="C27" t="n">
-        <v>8.59958061592936</v>
+        <v>4.66398638268545</v>
       </c>
     </row>
     <row r="28">
@@ -2137,7 +2137,7 @@
         <v>55</v>
       </c>
       <c r="C28" t="n">
-        <v>8.54661295935186</v>
+        <v>4.62668992607718</v>
       </c>
     </row>
     <row r="29">
@@ -2148,7 +2148,7 @@
         <v>55</v>
       </c>
       <c r="C29" t="n">
-        <v>8.48795510416641</v>
+        <v>4.52117871038361</v>
       </c>
     </row>
     <row r="30">
@@ -2159,7 +2159,7 @@
         <v>55</v>
       </c>
       <c r="C30" t="n">
-        <v>8.04359345056639</v>
+        <v>4.45077268543864</v>
       </c>
     </row>
     <row r="31">
@@ -2170,7 +2170,7 @@
         <v>55</v>
       </c>
       <c r="C31" t="n">
-        <v>7.97965648866054</v>
+        <v>4.34062147992938</v>
       </c>
     </row>
     <row r="32">
@@ -2181,7 +2181,7 @@
         <v>55</v>
       </c>
       <c r="C32" t="n">
-        <v>7.89028027630529</v>
+        <v>4.14611047976632</v>
       </c>
     </row>
     <row r="33">
@@ -2192,7 +2192,7 @@
         <v>55</v>
       </c>
       <c r="C33" t="n">
-        <v>7.64541166276007</v>
+        <v>4.09460353231631</v>
       </c>
     </row>
     <row r="34">
@@ -2203,7 +2203,7 @@
         <v>55</v>
       </c>
       <c r="C34" t="n">
-        <v>7.52597615307125</v>
+        <v>4.01464976516069</v>
       </c>
     </row>
     <row r="35">
@@ -2214,7 +2214,7 @@
         <v>55</v>
       </c>
       <c r="C35" t="n">
-        <v>7.51905980152944</v>
+        <v>3.9229543487363</v>
       </c>
     </row>
     <row r="36">
@@ -2225,7 +2225,7 @@
         <v>55</v>
       </c>
       <c r="C36" t="n">
-        <v>7.50953711164631</v>
+        <v>3.89928864576737</v>
       </c>
     </row>
     <row r="37">
@@ -2236,7 +2236,7 @@
         <v>55</v>
       </c>
       <c r="C37" t="n">
-        <v>7.37212165501504</v>
+        <v>3.87987282998086</v>
       </c>
     </row>
     <row r="38">
@@ -2247,7 +2247,7 @@
         <v>55</v>
       </c>
       <c r="C38" t="n">
-        <v>7.22175169038469</v>
+        <v>3.82062952420465</v>
       </c>
     </row>
     <row r="39">
@@ -2258,7 +2258,7 @@
         <v>55</v>
       </c>
       <c r="C39" t="n">
-        <v>7.12170677735484</v>
+        <v>3.81284602535527</v>
       </c>
     </row>
     <row r="40">
@@ -2269,7 +2269,7 @@
         <v>55</v>
       </c>
       <c r="C40" t="n">
-        <v>7.0576460297627</v>
+        <v>3.80784403009678</v>
       </c>
     </row>
     <row r="41">
@@ -2280,7 +2280,7 @@
         <v>55</v>
       </c>
       <c r="C41" t="n">
-        <v>6.94103404885495</v>
+        <v>3.7342073725184</v>
       </c>
     </row>
     <row r="42">
@@ -2291,7 +2291,7 @@
         <v>55</v>
       </c>
       <c r="C42" t="n">
-        <v>6.92484022436982</v>
+        <v>3.69107392271429</v>
       </c>
     </row>
     <row r="43">
@@ -2302,7 +2302,7 @@
         <v>55</v>
       </c>
       <c r="C43" t="n">
-        <v>6.8064376363933</v>
+        <v>3.44502456231606</v>
       </c>
     </row>
     <row r="44">
@@ -2313,7 +2313,7 @@
         <v>55</v>
       </c>
       <c r="C44" t="n">
-        <v>6.70040366623514</v>
+        <v>3.37548269312226</v>
       </c>
     </row>
     <row r="45">
@@ -2324,7 +2324,7 @@
         <v>55</v>
       </c>
       <c r="C45" t="n">
-        <v>6.64821846730171</v>
+        <v>3.32111068218545</v>
       </c>
     </row>
     <row r="46">
@@ -2335,7 +2335,7 @@
         <v>55</v>
       </c>
       <c r="C46" t="n">
-        <v>6.57462737718763</v>
+        <v>3.22051383104199</v>
       </c>
     </row>
     <row r="47">
@@ -2346,7 +2346,7 @@
         <v>55</v>
       </c>
       <c r="C47" t="n">
-        <v>6.53460168572225</v>
+        <v>3.16639729094708</v>
       </c>
     </row>
     <row r="48">
@@ -2357,7 +2357,7 @@
         <v>55</v>
       </c>
       <c r="C48" t="n">
-        <v>6.34503108997915</v>
+        <v>3.01656696555549</v>
       </c>
     </row>
     <row r="49">
@@ -2368,7 +2368,7 @@
         <v>55</v>
       </c>
       <c r="C49" t="n">
-        <v>6.28178419437802</v>
+        <v>3.01434562811356</v>
       </c>
     </row>
     <row r="50">
@@ -2379,7 +2379,7 @@
         <v>55</v>
       </c>
       <c r="C50" t="n">
-        <v>6.17023953537227</v>
+        <v>2.97342799225075</v>
       </c>
     </row>
     <row r="51">
@@ -2390,7 +2390,7 @@
         <v>55</v>
       </c>
       <c r="C51" t="n">
-        <v>6.01405769135519</v>
+        <v>2.97247490207117</v>
       </c>
     </row>
   </sheetData>
@@ -2426,7 +2426,7 @@
         <v>106</v>
       </c>
       <c r="C2" t="n">
-        <v>62.1538495403519</v>
+        <v>37.0157610122735</v>
       </c>
     </row>
     <row r="3">
@@ -2437,7 +2437,7 @@
         <v>106</v>
       </c>
       <c r="C3" t="n">
-        <v>58.7248431407743</v>
+        <v>34.6562588750203</v>
       </c>
     </row>
     <row r="4">
@@ -2448,7 +2448,7 @@
         <v>106</v>
       </c>
       <c r="C4" t="n">
-        <v>58.0147216175599</v>
+        <v>34.2169826769669</v>
       </c>
     </row>
     <row r="5">
@@ -2459,7 +2459,7 @@
         <v>106</v>
       </c>
       <c r="C5" t="n">
-        <v>56.6903131409388</v>
+        <v>32.6813099361196</v>
       </c>
     </row>
     <row r="6">
@@ -2470,7 +2470,7 @@
         <v>106</v>
       </c>
       <c r="C6" t="n">
-        <v>53.8637970247846</v>
+        <v>30.2555775322158</v>
       </c>
     </row>
     <row r="7">
@@ -2481,7 +2481,7 @@
         <v>106</v>
       </c>
       <c r="C7" t="n">
-        <v>52.0872033721583</v>
+        <v>30.1735261190558</v>
       </c>
     </row>
     <row r="8">
@@ -2492,7 +2492,7 @@
         <v>106</v>
       </c>
       <c r="C8" t="n">
-        <v>49.4987402571391</v>
+        <v>29.3682366661371</v>
       </c>
     </row>
     <row r="9">
@@ -2503,7 +2503,7 @@
         <v>106</v>
       </c>
       <c r="C9" t="n">
-        <v>47.1548102853547</v>
+        <v>27.2276547649188</v>
       </c>
     </row>
     <row r="10">
@@ -2514,7 +2514,7 @@
         <v>106</v>
       </c>
       <c r="C10" t="n">
-        <v>46.407596188088</v>
+        <v>26.1301945265918</v>
       </c>
     </row>
     <row r="11">
@@ -2525,7 +2525,7 @@
         <v>106</v>
       </c>
       <c r="C11" t="n">
-        <v>46.2184154615278</v>
+        <v>25.6478143688106</v>
       </c>
     </row>
     <row r="12">
@@ -2536,7 +2536,7 @@
         <v>106</v>
       </c>
       <c r="C12" t="n">
-        <v>45.6007919643246</v>
+        <v>25.3015733347148</v>
       </c>
     </row>
     <row r="13">
@@ -2547,7 +2547,7 @@
         <v>106</v>
       </c>
       <c r="C13" t="n">
-        <v>44.5323954949952</v>
+        <v>24.6619661415914</v>
       </c>
     </row>
     <row r="14">
@@ -2558,7 +2558,7 @@
         <v>106</v>
       </c>
       <c r="C14" t="n">
-        <v>44.2458771573619</v>
+        <v>24.2154144621845</v>
       </c>
     </row>
     <row r="15">
@@ -2569,7 +2569,7 @@
         <v>106</v>
       </c>
       <c r="C15" t="n">
-        <v>43.3667726433447</v>
+        <v>24.2098711530867</v>
       </c>
     </row>
     <row r="16">
@@ -2580,7 +2580,7 @@
         <v>106</v>
       </c>
       <c r="C16" t="n">
-        <v>43.2351044529236</v>
+        <v>24.1580984260729</v>
       </c>
     </row>
     <row r="17">
@@ -2591,7 +2591,7 @@
         <v>106</v>
       </c>
       <c r="C17" t="n">
-        <v>43.214597684043</v>
+        <v>23.7539239531983</v>
       </c>
     </row>
     <row r="18">
@@ -2602,7 +2602,7 @@
         <v>106</v>
       </c>
       <c r="C18" t="n">
-        <v>43.0060295887036</v>
+        <v>23.6937714731032</v>
       </c>
     </row>
     <row r="19">
@@ -2613,7 +2613,7 @@
         <v>106</v>
       </c>
       <c r="C19" t="n">
-        <v>42.9188724358195</v>
+        <v>23.379093335391</v>
       </c>
     </row>
     <row r="20">
@@ -2624,7 +2624,7 @@
         <v>106</v>
       </c>
       <c r="C20" t="n">
-        <v>42.8965623842</v>
+        <v>23.2806681392436</v>
       </c>
     </row>
     <row r="21">
@@ -2635,7 +2635,7 @@
         <v>106</v>
       </c>
       <c r="C21" t="n">
-        <v>42.6288901389397</v>
+        <v>23.1991610836394</v>
       </c>
     </row>
     <row r="22">
@@ -2646,7 +2646,7 @@
         <v>106</v>
       </c>
       <c r="C22" t="n">
-        <v>42.4210923951039</v>
+        <v>23.0533832022195</v>
       </c>
     </row>
     <row r="23">
@@ -2657,7 +2657,7 @@
         <v>106</v>
       </c>
       <c r="C23" t="n">
-        <v>42.1607617574845</v>
+        <v>23.032576577449</v>
       </c>
     </row>
     <row r="24">
@@ -2668,7 +2668,7 @@
         <v>106</v>
       </c>
       <c r="C24" t="n">
-        <v>41.7869725633981</v>
+        <v>22.8717421311274</v>
       </c>
     </row>
     <row r="25">
@@ -2679,7 +2679,7 @@
         <v>106</v>
       </c>
       <c r="C25" t="n">
-        <v>41.6176603773998</v>
+        <v>22.6989264317838</v>
       </c>
     </row>
     <row r="26">
@@ -2690,7 +2690,7 @@
         <v>106</v>
       </c>
       <c r="C26" t="n">
-        <v>41.4809206563847</v>
+        <v>22.6661110033697</v>
       </c>
     </row>
     <row r="27">
@@ -2701,7 +2701,7 @@
         <v>106</v>
       </c>
       <c r="C27" t="n">
-        <v>41.4693338848651</v>
+        <v>22.4879079844902</v>
       </c>
     </row>
     <row r="28">
@@ -2712,7 +2712,7 @@
         <v>106</v>
       </c>
       <c r="C28" t="n">
-        <v>41.3859101023049</v>
+        <v>22.0624707252455</v>
       </c>
     </row>
     <row r="29">
@@ -2723,7 +2723,7 @@
         <v>106</v>
       </c>
       <c r="C29" t="n">
-        <v>41.1145990206572</v>
+        <v>21.7257643832835</v>
       </c>
     </row>
     <row r="30">
@@ -2734,7 +2734,7 @@
         <v>106</v>
       </c>
       <c r="C30" t="n">
-        <v>40.6030078378051</v>
+        <v>21.2242301335926</v>
       </c>
     </row>
     <row r="31">
@@ -2745,7 +2745,7 @@
         <v>106</v>
       </c>
       <c r="C31" t="n">
-        <v>40.397888918381</v>
+        <v>21.0778463900129</v>
       </c>
     </row>
     <row r="32">
@@ -2756,7 +2756,7 @@
         <v>106</v>
       </c>
       <c r="C32" t="n">
-        <v>39.4736336595303</v>
+        <v>21.044048360849</v>
       </c>
     </row>
     <row r="33">
@@ -2767,7 +2767,7 @@
         <v>106</v>
       </c>
       <c r="C33" t="n">
-        <v>39.2568652637694</v>
+        <v>20.9741199727065</v>
       </c>
     </row>
     <row r="34">
@@ -2778,7 +2778,7 @@
         <v>106</v>
       </c>
       <c r="C34" t="n">
-        <v>38.7024475348565</v>
+        <v>20.8545599377166</v>
       </c>
     </row>
     <row r="35">
@@ -2789,7 +2789,7 @@
         <v>106</v>
       </c>
       <c r="C35" t="n">
-        <v>38.2193127897809</v>
+        <v>20.8169847552647</v>
       </c>
     </row>
     <row r="36">
@@ -2800,7 +2800,7 @@
         <v>106</v>
       </c>
       <c r="C36" t="n">
-        <v>38.1301095492767</v>
+        <v>20.7573350938284</v>
       </c>
     </row>
     <row r="37">
@@ -2811,7 +2811,7 @@
         <v>106</v>
       </c>
       <c r="C37" t="n">
-        <v>38.1010724053959</v>
+        <v>20.3168609737467</v>
       </c>
     </row>
     <row r="38">
@@ -2822,7 +2822,7 @@
         <v>106</v>
       </c>
       <c r="C38" t="n">
-        <v>37.9713844135663</v>
+        <v>20.1049947754161</v>
       </c>
     </row>
     <row r="39">
@@ -2833,7 +2833,7 @@
         <v>106</v>
       </c>
       <c r="C39" t="n">
-        <v>37.7481437914424</v>
+        <v>20.0049739629509</v>
       </c>
     </row>
     <row r="40">
@@ -2844,7 +2844,7 @@
         <v>106</v>
       </c>
       <c r="C40" t="n">
-        <v>37.5031829360793</v>
+        <v>19.9598772073484</v>
       </c>
     </row>
     <row r="41">
@@ -2855,7 +2855,7 @@
         <v>106</v>
       </c>
       <c r="C41" t="n">
-        <v>37.3331055361661</v>
+        <v>19.8732314086094</v>
       </c>
     </row>
     <row r="42">
@@ -2866,7 +2866,7 @@
         <v>106</v>
       </c>
       <c r="C42" t="n">
-        <v>37.0408197854601</v>
+        <v>19.5269193301287</v>
       </c>
     </row>
     <row r="43">
@@ -2877,7 +2877,7 @@
         <v>106</v>
       </c>
       <c r="C43" t="n">
-        <v>36.9834011724515</v>
+        <v>19.4055250890072</v>
       </c>
     </row>
     <row r="44">
@@ -2888,7 +2888,7 @@
         <v>106</v>
       </c>
       <c r="C44" t="n">
-        <v>36.6633634734035</v>
+        <v>19.2046423941761</v>
       </c>
     </row>
     <row r="45">
@@ -2899,7 +2899,7 @@
         <v>106</v>
       </c>
       <c r="C45" t="n">
-        <v>36.5909959084799</v>
+        <v>19.163227274608</v>
       </c>
     </row>
     <row r="46">
@@ -2910,7 +2910,7 @@
         <v>106</v>
       </c>
       <c r="C46" t="n">
-        <v>36.4962288365316</v>
+        <v>19.1282702315125</v>
       </c>
     </row>
     <row r="47">
@@ -2921,7 +2921,7 @@
         <v>106</v>
       </c>
       <c r="C47" t="n">
-        <v>36.1964940633786</v>
+        <v>19.0902023453529</v>
       </c>
     </row>
     <row r="48">
@@ -2932,7 +2932,7 @@
         <v>106</v>
       </c>
       <c r="C48" t="n">
-        <v>36.0506400266298</v>
+        <v>18.4356440280405</v>
       </c>
     </row>
     <row r="49">
@@ -2943,7 +2943,7 @@
         <v>106</v>
       </c>
       <c r="C49" t="n">
-        <v>35.9453807686276</v>
+        <v>18.4348447109633</v>
       </c>
     </row>
     <row r="50">
@@ -2954,7 +2954,7 @@
         <v>106</v>
       </c>
       <c r="C50" t="n">
-        <v>35.4103464672598</v>
+        <v>18.384690159223</v>
       </c>
     </row>
     <row r="51">
@@ -2965,7 +2965,7 @@
         <v>106</v>
       </c>
       <c r="C51" t="n">
-        <v>35.1797835463309</v>
+        <v>18.2733150446718</v>
       </c>
     </row>
   </sheetData>
@@ -3001,7 +3001,7 @@
         <v>157</v>
       </c>
       <c r="C2" t="n">
-        <v>20.1553694938929</v>
+        <v>11.4920564464015</v>
       </c>
     </row>
     <row r="3">
@@ -3012,7 +3012,7 @@
         <v>157</v>
       </c>
       <c r="C3" t="n">
-        <v>19.1842806618586</v>
+        <v>11.4406109667859</v>
       </c>
     </row>
     <row r="4">
@@ -3023,7 +3023,7 @@
         <v>157</v>
       </c>
       <c r="C4" t="n">
-        <v>19.1281077612218</v>
+        <v>10.8096774412675</v>
       </c>
     </row>
     <row r="5">
@@ -3034,7 +3034,7 @@
         <v>157</v>
       </c>
       <c r="C5" t="n">
-        <v>18.9589105399885</v>
+        <v>10.5800942186318</v>
       </c>
     </row>
     <row r="6">
@@ -3045,7 +3045,7 @@
         <v>157</v>
       </c>
       <c r="C6" t="n">
-        <v>17.1488407992269</v>
+        <v>9.90351743492169</v>
       </c>
     </row>
     <row r="7">
@@ -3056,7 +3056,7 @@
         <v>157</v>
       </c>
       <c r="C7" t="n">
-        <v>17.0346635926954</v>
+        <v>9.34634960938037</v>
       </c>
     </row>
     <row r="8">
@@ -3067,7 +3067,7 @@
         <v>157</v>
       </c>
       <c r="C8" t="n">
-        <v>16.881357556406</v>
+        <v>9.21936731110615</v>
       </c>
     </row>
     <row r="9">
@@ -3078,7 +3078,7 @@
         <v>157</v>
       </c>
       <c r="C9" t="n">
-        <v>15.7582772567992</v>
+        <v>8.48256060778412</v>
       </c>
     </row>
     <row r="10">
@@ -3089,7 +3089,7 @@
         <v>157</v>
       </c>
       <c r="C10" t="n">
-        <v>15.6853237152335</v>
+        <v>8.48091490693891</v>
       </c>
     </row>
     <row r="11">
@@ -3100,7 +3100,7 @@
         <v>157</v>
       </c>
       <c r="C11" t="n">
-        <v>15.1509657165313</v>
+        <v>8.37522186703904</v>
       </c>
     </row>
     <row r="12">
@@ -3111,7 +3111,7 @@
         <v>157</v>
       </c>
       <c r="C12" t="n">
-        <v>14.4200453496968</v>
+        <v>7.77401497515537</v>
       </c>
     </row>
     <row r="13">
@@ -3122,7 +3122,7 @@
         <v>157</v>
       </c>
       <c r="C13" t="n">
-        <v>14.1044352395306</v>
+        <v>7.73102749304711</v>
       </c>
     </row>
     <row r="14">
@@ -3133,7 +3133,7 @@
         <v>157</v>
       </c>
       <c r="C14" t="n">
-        <v>13.6854422341073</v>
+        <v>7.46402598705246</v>
       </c>
     </row>
     <row r="15">
@@ -3144,7 +3144,7 @@
         <v>157</v>
       </c>
       <c r="C15" t="n">
-        <v>13.653975362347</v>
+        <v>7.32991396718563</v>
       </c>
     </row>
     <row r="16">
@@ -3155,7 +3155,7 @@
         <v>157</v>
       </c>
       <c r="C16" t="n">
-        <v>13.5788104251161</v>
+        <v>7.08258516241405</v>
       </c>
     </row>
     <row r="17">
@@ -3166,7 +3166,7 @@
         <v>157</v>
       </c>
       <c r="C17" t="n">
-        <v>13.3973505486418</v>
+        <v>7.07433731496416</v>
       </c>
     </row>
     <row r="18">
@@ -3177,7 +3177,7 @@
         <v>157</v>
       </c>
       <c r="C18" t="n">
-        <v>12.7674435911509</v>
+        <v>6.97823395008623</v>
       </c>
     </row>
     <row r="19">
@@ -3188,7 +3188,7 @@
         <v>157</v>
       </c>
       <c r="C19" t="n">
-        <v>12.617992073571</v>
+        <v>6.94774095829247</v>
       </c>
     </row>
     <row r="20">
@@ -3199,7 +3199,7 @@
         <v>157</v>
       </c>
       <c r="C20" t="n">
-        <v>12.1004468004031</v>
+        <v>6.0741120023142</v>
       </c>
     </row>
     <row r="21">
@@ -3210,7 +3210,7 @@
         <v>157</v>
       </c>
       <c r="C21" t="n">
-        <v>11.9141770700275</v>
+        <v>6.00061121943595</v>
       </c>
     </row>
     <row r="22">
@@ -3221,7 +3221,7 @@
         <v>157</v>
       </c>
       <c r="C22" t="n">
-        <v>11.6836003416138</v>
+        <v>5.75472161787257</v>
       </c>
     </row>
     <row r="23">
@@ -3232,7 +3232,7 @@
         <v>157</v>
       </c>
       <c r="C23" t="n">
-        <v>11.3312600410793</v>
+        <v>5.74747075707391</v>
       </c>
     </row>
     <row r="24">
@@ -3243,7 +3243,7 @@
         <v>157</v>
       </c>
       <c r="C24" t="n">
-        <v>11.2508886064411</v>
+        <v>5.58692931921574</v>
       </c>
     </row>
     <row r="25">
@@ -3254,7 +3254,7 @@
         <v>157</v>
       </c>
       <c r="C25" t="n">
-        <v>11.0195424578049</v>
+        <v>5.56018202110882</v>
       </c>
     </row>
     <row r="26">
@@ -3265,7 +3265,7 @@
         <v>157</v>
       </c>
       <c r="C26" t="n">
-        <v>11.0100295067028</v>
+        <v>5.5393856960907</v>
       </c>
     </row>
     <row r="27">
@@ -3276,7 +3276,7 @@
         <v>157</v>
       </c>
       <c r="C27" t="n">
-        <v>11.0006965191389</v>
+        <v>5.44116809628675</v>
       </c>
     </row>
     <row r="28">
@@ -3287,7 +3287,7 @@
         <v>157</v>
       </c>
       <c r="C28" t="n">
-        <v>10.9166259386074</v>
+        <v>5.41110856316418</v>
       </c>
     </row>
     <row r="29">
@@ -3298,7 +3298,7 @@
         <v>157</v>
       </c>
       <c r="C29" t="n">
-        <v>10.8114657701255</v>
+        <v>5.29681038815191</v>
       </c>
     </row>
     <row r="30">
@@ -3309,7 +3309,7 @@
         <v>157</v>
       </c>
       <c r="C30" t="n">
-        <v>10.6524700142992</v>
+        <v>5.05345635572691</v>
       </c>
     </row>
     <row r="31">
@@ -3320,7 +3320,7 @@
         <v>157</v>
       </c>
       <c r="C31" t="n">
-        <v>10.6143430684066</v>
+        <v>5.04445914985704</v>
       </c>
     </row>
     <row r="32">
@@ -3331,7 +3331,7 @@
         <v>157</v>
       </c>
       <c r="C32" t="n">
-        <v>10.5138213953198</v>
+        <v>5.03276051252334</v>
       </c>
     </row>
     <row r="33">
@@ -3342,7 +3342,7 @@
         <v>157</v>
       </c>
       <c r="C33" t="n">
-        <v>10.2079365287378</v>
+        <v>4.99443035389798</v>
       </c>
     </row>
     <row r="34">
@@ -3353,7 +3353,7 @@
         <v>157</v>
       </c>
       <c r="C34" t="n">
-        <v>10.0108293471106</v>
+        <v>4.88915578033663</v>
       </c>
     </row>
     <row r="35">
@@ -3364,7 +3364,7 @@
         <v>157</v>
       </c>
       <c r="C35" t="n">
-        <v>9.85129033480747</v>
+        <v>4.78196212440119</v>
       </c>
     </row>
     <row r="36">
@@ -3375,7 +3375,7 @@
         <v>157</v>
       </c>
       <c r="C36" t="n">
-        <v>9.80275820653016</v>
+        <v>4.74733208330638</v>
       </c>
     </row>
     <row r="37">
@@ -3386,7 +3386,7 @@
         <v>157</v>
       </c>
       <c r="C37" t="n">
-        <v>9.78957291106555</v>
+        <v>4.66421052242338</v>
       </c>
     </row>
     <row r="38">
@@ -3397,7 +3397,7 @@
         <v>157</v>
       </c>
       <c r="C38" t="n">
-        <v>9.6588078444809</v>
+        <v>4.61648689480515</v>
       </c>
     </row>
     <row r="39">
@@ -3408,7 +3408,7 @@
         <v>157</v>
       </c>
       <c r="C39" t="n">
-        <v>9.65366369597719</v>
+        <v>4.60112968138155</v>
       </c>
     </row>
     <row r="40">
@@ -3419,7 +3419,7 @@
         <v>157</v>
       </c>
       <c r="C40" t="n">
-        <v>9.58992492114078</v>
+        <v>4.44648267928174</v>
       </c>
     </row>
     <row r="41">
@@ -3430,7 +3430,7 @@
         <v>157</v>
       </c>
       <c r="C41" t="n">
-        <v>9.40216958795883</v>
+        <v>4.36798297714091</v>
       </c>
     </row>
     <row r="42">
@@ -3441,7 +3441,7 @@
         <v>157</v>
       </c>
       <c r="C42" t="n">
-        <v>9.33061164346441</v>
+        <v>4.36079892584063</v>
       </c>
     </row>
     <row r="43">
@@ -3452,7 +3452,7 @@
         <v>157</v>
       </c>
       <c r="C43" t="n">
-        <v>8.95285826309761</v>
+        <v>4.30741044276686</v>
       </c>
     </row>
     <row r="44">
@@ -3463,7 +3463,7 @@
         <v>157</v>
       </c>
       <c r="C44" t="n">
-        <v>8.91708344135026</v>
+        <v>4.28673773267988</v>
       </c>
     </row>
     <row r="45">
@@ -3474,7 +3474,7 @@
         <v>157</v>
       </c>
       <c r="C45" t="n">
-        <v>8.75513259770999</v>
+        <v>4.06342550184901</v>
       </c>
     </row>
     <row r="46">
@@ -3485,7 +3485,7 @@
         <v>157</v>
       </c>
       <c r="C46" t="n">
-        <v>8.68469892377011</v>
+        <v>4.03716051106119</v>
       </c>
     </row>
     <row r="47">
@@ -3496,7 +3496,7 @@
         <v>157</v>
       </c>
       <c r="C47" t="n">
-        <v>8.68185876886248</v>
+        <v>3.81971661096978</v>
       </c>
     </row>
     <row r="48">
@@ -3507,7 +3507,7 @@
         <v>157</v>
       </c>
       <c r="C48" t="n">
-        <v>8.47546411854971</v>
+        <v>3.76058093095948</v>
       </c>
     </row>
     <row r="49">
@@ -3518,7 +3518,7 @@
         <v>157</v>
       </c>
       <c r="C49" t="n">
-        <v>8.41216624079178</v>
+        <v>3.73550653344454</v>
       </c>
     </row>
     <row r="50">
@@ -3529,7 +3529,7 @@
         <v>157</v>
       </c>
       <c r="C50" t="n">
-        <v>8.38298066902974</v>
+        <v>3.73479354273561</v>
       </c>
     </row>
     <row r="51">
@@ -3540,7 +3540,7 @@
         <v>157</v>
       </c>
       <c r="C51" t="n">
-        <v>8.30780647075059</v>
+        <v>3.59257874375825</v>
       </c>
     </row>
   </sheetData>
@@ -3576,7 +3576,7 @@
         <v>208</v>
       </c>
       <c r="C2" t="n">
-        <v>57.4323814738256</v>
+        <v>41.6696749144394</v>
       </c>
     </row>
     <row r="3">
@@ -3587,7 +3587,7 @@
         <v>208</v>
       </c>
       <c r="C3" t="n">
-        <v>57.2335527911267</v>
+        <v>41.194245990759</v>
       </c>
     </row>
     <row r="4">
@@ -3598,7 +3598,7 @@
         <v>208</v>
       </c>
       <c r="C4" t="n">
-        <v>57.096714254952</v>
+        <v>40.6759461149655</v>
       </c>
     </row>
     <row r="5">
@@ -3609,7 +3609,7 @@
         <v>208</v>
       </c>
       <c r="C5" t="n">
-        <v>56.3928853423078</v>
+        <v>40.3985846582526</v>
       </c>
     </row>
     <row r="6">
@@ -3620,7 +3620,7 @@
         <v>208</v>
       </c>
       <c r="C6" t="n">
-        <v>54.3606019099296</v>
+        <v>38.1706268106365</v>
       </c>
     </row>
     <row r="7">
@@ -3631,7 +3631,7 @@
         <v>208</v>
       </c>
       <c r="C7" t="n">
-        <v>53.655914724711</v>
+        <v>37.6234853549002</v>
       </c>
     </row>
     <row r="8">
@@ -3642,7 +3642,7 @@
         <v>208</v>
       </c>
       <c r="C8" t="n">
-        <v>53.5458286588195</v>
+        <v>37.2625552409209</v>
       </c>
     </row>
     <row r="9">
@@ -3653,7 +3653,7 @@
         <v>208</v>
       </c>
       <c r="C9" t="n">
-        <v>52.711883239475</v>
+        <v>36.9721038587947</v>
       </c>
     </row>
     <row r="10">
@@ -3664,7 +3664,7 @@
         <v>208</v>
       </c>
       <c r="C10" t="n">
-        <v>51.9112118898725</v>
+        <v>36.0874928225477</v>
       </c>
     </row>
     <row r="11">
@@ -3675,7 +3675,7 @@
         <v>208</v>
       </c>
       <c r="C11" t="n">
-        <v>50.7367563397472</v>
+        <v>35.2962974969455</v>
       </c>
     </row>
     <row r="12">
@@ -3686,7 +3686,7 @@
         <v>208</v>
       </c>
       <c r="C12" t="n">
-        <v>50.4400434856151</v>
+        <v>35.0362043633793</v>
       </c>
     </row>
     <row r="13">
@@ -3697,7 +3697,7 @@
         <v>208</v>
       </c>
       <c r="C13" t="n">
-        <v>50.3485557954433</v>
+        <v>34.8664191097166</v>
       </c>
     </row>
     <row r="14">
@@ -3708,7 +3708,7 @@
         <v>208</v>
       </c>
       <c r="C14" t="n">
-        <v>50.1056325614171</v>
+        <v>34.4436903770818</v>
       </c>
     </row>
     <row r="15">
@@ -3719,7 +3719,7 @@
         <v>208</v>
       </c>
       <c r="C15" t="n">
-        <v>49.9807926996004</v>
+        <v>34.4217655390834</v>
       </c>
     </row>
     <row r="16">
@@ -3730,7 +3730,7 @@
         <v>208</v>
       </c>
       <c r="C16" t="n">
-        <v>49.381445521953</v>
+        <v>34.0732471197392</v>
       </c>
     </row>
     <row r="17">
@@ -3741,7 +3741,7 @@
         <v>208</v>
       </c>
       <c r="C17" t="n">
-        <v>49.3711919151977</v>
+        <v>33.7050600772296</v>
       </c>
     </row>
     <row r="18">
@@ -3752,7 +3752,7 @@
         <v>208</v>
       </c>
       <c r="C18" t="n">
-        <v>49.2087294372716</v>
+        <v>33.6774529246831</v>
       </c>
     </row>
     <row r="19">
@@ -3763,7 +3763,7 @@
         <v>208</v>
       </c>
       <c r="C19" t="n">
-        <v>49.1221842468728</v>
+        <v>33.4438515467657</v>
       </c>
     </row>
     <row r="20">
@@ -3774,7 +3774,7 @@
         <v>208</v>
       </c>
       <c r="C20" t="n">
-        <v>48.9397699675805</v>
+        <v>33.4033048352342</v>
       </c>
     </row>
     <row r="21">
@@ -3785,7 +3785,7 @@
         <v>208</v>
       </c>
       <c r="C21" t="n">
-        <v>48.2810475551503</v>
+        <v>32.8805027045904</v>
       </c>
     </row>
     <row r="22">
@@ -3796,7 +3796,7 @@
         <v>208</v>
       </c>
       <c r="C22" t="n">
-        <v>47.9382059520351</v>
+        <v>32.8773760734444</v>
       </c>
     </row>
     <row r="23">
@@ -3807,7 +3807,7 @@
         <v>208</v>
       </c>
       <c r="C23" t="n">
-        <v>47.4236490846586</v>
+        <v>32.6881513783219</v>
       </c>
     </row>
     <row r="24">
@@ -3818,7 +3818,7 @@
         <v>208</v>
       </c>
       <c r="C24" t="n">
-        <v>47.3595692614863</v>
+        <v>32.4961542829696</v>
       </c>
     </row>
     <row r="25">
@@ -3829,7 +3829,7 @@
         <v>208</v>
       </c>
       <c r="C25" t="n">
-        <v>47.3406134860467</v>
+        <v>32.1485926088568</v>
       </c>
     </row>
     <row r="26">
@@ -3840,7 +3840,7 @@
         <v>208</v>
       </c>
       <c r="C26" t="n">
-        <v>46.6823258385851</v>
+        <v>31.3096625723559</v>
       </c>
     </row>
     <row r="27">
@@ -3851,7 +3851,7 @@
         <v>208</v>
       </c>
       <c r="C27" t="n">
-        <v>46.6487917657576</v>
+        <v>30.9054239207572</v>
       </c>
     </row>
     <row r="28">
@@ -3862,7 +3862,7 @@
         <v>208</v>
       </c>
       <c r="C28" t="n">
-        <v>45.6836383348171</v>
+        <v>30.7724563945192</v>
       </c>
     </row>
     <row r="29">
@@ -3873,7 +3873,7 @@
         <v>208</v>
       </c>
       <c r="C29" t="n">
-        <v>45.6277258184648</v>
+        <v>30.7349534419192</v>
       </c>
     </row>
     <row r="30">
@@ -3884,7 +3884,7 @@
         <v>208</v>
       </c>
       <c r="C30" t="n">
-        <v>45.3372350389106</v>
+        <v>30.3202219769659</v>
       </c>
     </row>
     <row r="31">
@@ -3895,7 +3895,7 @@
         <v>208</v>
       </c>
       <c r="C31" t="n">
-        <v>44.9572438050495</v>
+        <v>30.2725955896988</v>
       </c>
     </row>
     <row r="32">
@@ -3906,7 +3906,7 @@
         <v>208</v>
       </c>
       <c r="C32" t="n">
-        <v>44.2120668463059</v>
+        <v>30.0349501167409</v>
       </c>
     </row>
     <row r="33">
@@ -3917,7 +3917,7 @@
         <v>208</v>
       </c>
       <c r="C33" t="n">
-        <v>43.9751499668748</v>
+        <v>29.7854156056487</v>
       </c>
     </row>
     <row r="34">
@@ -3928,7 +3928,7 @@
         <v>208</v>
       </c>
       <c r="C34" t="n">
-        <v>43.5370669054883</v>
+        <v>29.5632850701118</v>
       </c>
     </row>
     <row r="35">
@@ -3939,7 +3939,7 @@
         <v>208</v>
       </c>
       <c r="C35" t="n">
-        <v>43.5255660365023</v>
+        <v>29.1690044505505</v>
       </c>
     </row>
     <row r="36">
@@ -3950,7 +3950,7 @@
         <v>208</v>
       </c>
       <c r="C36" t="n">
-        <v>43.4369409202234</v>
+        <v>28.8205991328503</v>
       </c>
     </row>
     <row r="37">
@@ -3961,7 +3961,7 @@
         <v>208</v>
       </c>
       <c r="C37" t="n">
-        <v>42.8984251604745</v>
+        <v>28.528028663069</v>
       </c>
     </row>
     <row r="38">
@@ -3972,7 +3972,7 @@
         <v>208</v>
       </c>
       <c r="C38" t="n">
-        <v>42.3778056166909</v>
+        <v>28.5229684939802</v>
       </c>
     </row>
     <row r="39">
@@ -3983,7 +3983,7 @@
         <v>208</v>
       </c>
       <c r="C39" t="n">
-        <v>42.1771667154621</v>
+        <v>27.824858478157</v>
       </c>
     </row>
     <row r="40">
@@ -3994,7 +3994,7 @@
         <v>208</v>
       </c>
       <c r="C40" t="n">
-        <v>42.1579782423968</v>
+        <v>27.6869631705195</v>
       </c>
     </row>
     <row r="41">
@@ -4005,7 +4005,7 @@
         <v>208</v>
       </c>
       <c r="C41" t="n">
-        <v>41.9999924371744</v>
+        <v>27.6209591567959</v>
       </c>
     </row>
     <row r="42">
@@ -4016,7 +4016,7 @@
         <v>208</v>
       </c>
       <c r="C42" t="n">
-        <v>41.7438828770238</v>
+        <v>27.3756468368287</v>
       </c>
     </row>
     <row r="43">
@@ -4027,7 +4027,7 @@
         <v>208</v>
       </c>
       <c r="C43" t="n">
-        <v>41.252198726956</v>
+        <v>27.1393692758757</v>
       </c>
     </row>
     <row r="44">
@@ -4038,7 +4038,7 @@
         <v>208</v>
       </c>
       <c r="C44" t="n">
-        <v>40.8345551276346</v>
+        <v>26.6672913670585</v>
       </c>
     </row>
     <row r="45">
@@ -4049,7 +4049,7 @@
         <v>208</v>
       </c>
       <c r="C45" t="n">
-        <v>40.6404523121514</v>
+        <v>25.7597029787485</v>
       </c>
     </row>
     <row r="46">
@@ -4060,7 +4060,7 @@
         <v>208</v>
       </c>
       <c r="C46" t="n">
-        <v>39.3100237465931</v>
+        <v>25.7341244940757</v>
       </c>
     </row>
     <row r="47">
@@ -4071,7 +4071,7 @@
         <v>208</v>
       </c>
       <c r="C47" t="n">
-        <v>39.2144004520963</v>
+        <v>25.2117418636027</v>
       </c>
     </row>
     <row r="48">
@@ -4082,7 +4082,7 @@
         <v>208</v>
       </c>
       <c r="C48" t="n">
-        <v>38.7698387230867</v>
+        <v>24.9931516921233</v>
       </c>
     </row>
     <row r="49">
@@ -4093,7 +4093,7 @@
         <v>208</v>
       </c>
       <c r="C49" t="n">
-        <v>38.5805717792888</v>
+        <v>24.6452650875793</v>
       </c>
     </row>
     <row r="50">
@@ -4104,7 +4104,7 @@
         <v>208</v>
       </c>
       <c r="C50" t="n">
-        <v>38.0047297283871</v>
+        <v>24.6162410708441</v>
       </c>
     </row>
     <row r="51">
@@ -4115,7 +4115,7 @@
         <v>208</v>
       </c>
       <c r="C51" t="n">
-        <v>37.9471646613555</v>
+        <v>24.3809896669279</v>
       </c>
     </row>
   </sheetData>
@@ -4151,7 +4151,7 @@
         <v>259</v>
       </c>
       <c r="C2" t="n">
-        <v>9.20955129557698</v>
+        <v>6.27497458230458</v>
       </c>
     </row>
     <row r="3">
@@ -4162,7 +4162,7 @@
         <v>259</v>
       </c>
       <c r="C3" t="n">
-        <v>8.49864449920862</v>
+        <v>5.60735870082252</v>
       </c>
     </row>
     <row r="4">
@@ -4173,7 +4173,7 @@
         <v>259</v>
       </c>
       <c r="C4" t="n">
-        <v>7.885675056091</v>
+        <v>5.04377246484585</v>
       </c>
     </row>
     <row r="5">
@@ -4184,7 +4184,7 @@
         <v>259</v>
       </c>
       <c r="C5" t="n">
-        <v>7.12542959299041</v>
+        <v>4.49604956430223</v>
       </c>
     </row>
     <row r="6">
@@ -4195,7 +4195,7 @@
         <v>259</v>
       </c>
       <c r="C6" t="n">
-        <v>7.09235052600468</v>
+        <v>4.41452430491532</v>
       </c>
     </row>
     <row r="7">
@@ -4206,7 +4206,7 @@
         <v>259</v>
       </c>
       <c r="C7" t="n">
-        <v>6.60726381625989</v>
+        <v>4.11257254197386</v>
       </c>
     </row>
     <row r="8">
@@ -4217,7 +4217,7 @@
         <v>259</v>
       </c>
       <c r="C8" t="n">
-        <v>6.54814601813101</v>
+        <v>4.01279401873042</v>
       </c>
     </row>
     <row r="9">
@@ -4228,7 +4228,7 @@
         <v>259</v>
       </c>
       <c r="C9" t="n">
-        <v>6.03393989209703</v>
+        <v>3.74703921386315</v>
       </c>
     </row>
     <row r="10">
@@ -4239,7 +4239,7 @@
         <v>259</v>
       </c>
       <c r="C10" t="n">
-        <v>5.99861510099871</v>
+        <v>3.67070856921056</v>
       </c>
     </row>
     <row r="11">
@@ -4250,7 +4250,7 @@
         <v>259</v>
       </c>
       <c r="C11" t="n">
-        <v>5.81117875272571</v>
+        <v>3.53787533046704</v>
       </c>
     </row>
     <row r="12">
@@ -4261,7 +4261,7 @@
         <v>259</v>
       </c>
       <c r="C12" t="n">
-        <v>5.77105434483684</v>
+        <v>3.43208924781432</v>
       </c>
     </row>
     <row r="13">
@@ -4272,7 +4272,7 @@
         <v>259</v>
       </c>
       <c r="C13" t="n">
-        <v>4.97820801828443</v>
+        <v>2.88258977049173</v>
       </c>
     </row>
     <row r="14">
@@ -4283,7 +4283,7 @@
         <v>259</v>
       </c>
       <c r="C14" t="n">
-        <v>4.94681083710858</v>
+        <v>2.84115292043438</v>
       </c>
     </row>
     <row r="15">
@@ -4294,7 +4294,7 @@
         <v>259</v>
       </c>
       <c r="C15" t="n">
-        <v>4.83491484773405</v>
+        <v>2.79511012535633</v>
       </c>
     </row>
     <row r="16">
@@ -4305,7 +4305,7 @@
         <v>259</v>
       </c>
       <c r="C16" t="n">
-        <v>4.77399265010381</v>
+        <v>2.72941262529586</v>
       </c>
     </row>
     <row r="17">
@@ -4316,7 +4316,7 @@
         <v>259</v>
       </c>
       <c r="C17" t="n">
-        <v>4.22949634994166</v>
+        <v>2.21102273380305</v>
       </c>
     </row>
     <row r="18">
@@ -4327,7 +4327,7 @@
         <v>259</v>
       </c>
       <c r="C18" t="n">
-        <v>3.87941280310049</v>
+        <v>2.09152862739968</v>
       </c>
     </row>
     <row r="19">
@@ -4338,7 +4338,7 @@
         <v>259</v>
       </c>
       <c r="C19" t="n">
-        <v>3.71182628842529</v>
+        <v>1.93246387764342</v>
       </c>
     </row>
     <row r="20">
@@ -4349,7 +4349,7 @@
         <v>259</v>
       </c>
       <c r="C20" t="n">
-        <v>3.70066277823507</v>
+        <v>1.92208896587951</v>
       </c>
     </row>
     <row r="21">
@@ -4360,7 +4360,7 @@
         <v>259</v>
       </c>
       <c r="C21" t="n">
-        <v>3.53846735319246</v>
+        <v>1.84370276541197</v>
       </c>
     </row>
     <row r="22">
@@ -4371,7 +4371,7 @@
         <v>259</v>
       </c>
       <c r="C22" t="n">
-        <v>3.43060734246669</v>
+        <v>1.75582030796151</v>
       </c>
     </row>
     <row r="23">
@@ -4382,7 +4382,7 @@
         <v>259</v>
       </c>
       <c r="C23" t="n">
-        <v>3.33867177902259</v>
+        <v>1.71579552797469</v>
       </c>
     </row>
     <row r="24">
@@ -4393,7 +4393,7 @@
         <v>259</v>
       </c>
       <c r="C24" t="n">
-        <v>3.22526931232234</v>
+        <v>1.55091427975333</v>
       </c>
     </row>
     <row r="25">
@@ -4404,7 +4404,7 @@
         <v>259</v>
       </c>
       <c r="C25" t="n">
-        <v>3.13954707826933</v>
+        <v>1.52735178842917</v>
       </c>
     </row>
     <row r="26">
@@ -4415,7 +4415,7 @@
         <v>259</v>
       </c>
       <c r="C26" t="n">
-        <v>3.06498278391037</v>
+        <v>1.50904558981279</v>
       </c>
     </row>
     <row r="27">
@@ -4426,7 +4426,7 @@
         <v>259</v>
       </c>
       <c r="C27" t="n">
-        <v>3.03443235784442</v>
+        <v>1.42908308021559</v>
       </c>
     </row>
     <row r="28">
@@ -4437,7 +4437,7 @@
         <v>259</v>
       </c>
       <c r="C28" t="n">
-        <v>3.00847061559393</v>
+        <v>1.42623437343035</v>
       </c>
     </row>
     <row r="29">
@@ -4448,7 +4448,7 @@
         <v>259</v>
       </c>
       <c r="C29" t="n">
-        <v>2.71052919954957</v>
+        <v>1.26958000836212</v>
       </c>
     </row>
     <row r="30">
@@ -4459,7 +4459,7 @@
         <v>259</v>
       </c>
       <c r="C30" t="n">
-        <v>2.51171640149322</v>
+        <v>1.239022247926</v>
       </c>
     </row>
     <row r="31">
@@ -4470,7 +4470,7 @@
         <v>259</v>
       </c>
       <c r="C31" t="n">
-        <v>2.42188729573321</v>
+        <v>1.12216058437917</v>
       </c>
     </row>
     <row r="32">
@@ -4481,7 +4481,7 @@
         <v>259</v>
       </c>
       <c r="C32" t="n">
-        <v>2.36256142115352</v>
+        <v>1.12017082152254</v>
       </c>
     </row>
     <row r="33">
@@ -4492,7 +4492,7 @@
         <v>259</v>
       </c>
       <c r="C33" t="n">
-        <v>2.27720152972697</v>
+        <v>1.03081819636543</v>
       </c>
     </row>
     <row r="34">
@@ -4503,7 +4503,7 @@
         <v>259</v>
       </c>
       <c r="C34" t="n">
-        <v>2.07653381360439</v>
+        <v>0.965078498811467</v>
       </c>
     </row>
     <row r="35">
@@ -4514,7 +4514,7 @@
         <v>259</v>
       </c>
       <c r="C35" t="n">
-        <v>2.07025258968325</v>
+        <v>0.944396509825871</v>
       </c>
     </row>
     <row r="36">
@@ -4525,7 +4525,7 @@
         <v>259</v>
       </c>
       <c r="C36" t="n">
-        <v>1.74104731235573</v>
+        <v>0.753143583994873</v>
       </c>
     </row>
     <row r="37">
@@ -4536,7 +4536,7 @@
         <v>259</v>
       </c>
       <c r="C37" t="n">
-        <v>1.70769861086619</v>
+        <v>0.703900182479856</v>
       </c>
     </row>
     <row r="38">
@@ -4547,7 +4547,7 @@
         <v>259</v>
       </c>
       <c r="C38" t="n">
-        <v>1.60536261423775</v>
+        <v>0.642249904349538</v>
       </c>
     </row>
     <row r="39">
@@ -4558,7 +4558,7 @@
         <v>259</v>
       </c>
       <c r="C39" t="n">
-        <v>1.4927872463121</v>
+        <v>0.611385559238685</v>
       </c>
     </row>
     <row r="40">
@@ -4569,7 +4569,7 @@
         <v>259</v>
       </c>
       <c r="C40" t="n">
-        <v>1.41494795184635</v>
+        <v>0.584822484087515</v>
       </c>
     </row>
     <row r="41">
@@ -4580,7 +4580,7 @@
         <v>259</v>
       </c>
       <c r="C41" t="n">
-        <v>1.24414352806377</v>
+        <v>0.577372249604482</v>
       </c>
     </row>
     <row r="42">
@@ -4591,7 +4591,7 @@
         <v>259</v>
       </c>
       <c r="C42" t="n">
-        <v>1.13733426246516</v>
+        <v>0.489463527131775</v>
       </c>
     </row>
     <row r="43">
@@ -4602,7 +4602,7 @@
         <v>259</v>
       </c>
       <c r="C43" t="n">
-        <v>1.1333259417504</v>
+        <v>0.408368504928881</v>
       </c>
     </row>
     <row r="44">
@@ -4613,7 +4613,7 @@
         <v>259</v>
       </c>
       <c r="C44" t="n">
-        <v>0.809655382711449</v>
+        <v>0.288271054190385</v>
       </c>
     </row>
     <row r="45">
@@ -4624,7 +4624,7 @@
         <v>259</v>
       </c>
       <c r="C45" t="n">
-        <v>0.445953218823875</v>
+        <v>0.13264197018908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>